<commit_message>
a bit more ottr-data
</commit_message>
<xml_diff>
--- a/ottr/data.xlsx
+++ b/ottr/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/veronika_heimsbakk_capgemini_com/Documents/Offentlig sektor/Digdir hackathon/shacl/ottr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{579C6417-8798-4F31-9F4D-6BE1B00EC5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55D404C7-1985-431C-998E-03C12A71BE14}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{579C6417-8798-4F31-9F4D-6BE1B00EC5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60BED205-6AD0-4C2A-8C78-96DA9A64C37A}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D60C6248-8651-4F70-B11C-5F99C904C353}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D60C6248-8651-4F70-B11C-5F99C904C353}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
   <si>
     <t>prefix</t>
   </si>
@@ -167,13 +167,97 @@
   </si>
   <si>
     <t>AUDIENCE</t>
+  </si>
+  <si>
+    <t>ex:Deklarasjonspliktig</t>
+  </si>
+  <si>
+    <t>Deklarasjonspliktig@@nb</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d137</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d138</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d139</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d140</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d141</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d142</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d143</t>
+  </si>
+  <si>
+    <t>https://begrepskatalog.demo.fellesdatakatalog.digdir.no/555111097/f3274666-cce4-408f-ad2a-1569d242d144</t>
+  </si>
+  <si>
+    <t>ex:Deklarasjon</t>
+  </si>
+  <si>
+    <t>Deklarasjon@@nb</t>
+  </si>
+  <si>
+    <t>ex:Fartøy</t>
+  </si>
+  <si>
+    <t>Fartøy@@nb</t>
+  </si>
+  <si>
+    <t>ex:Fører</t>
+  </si>
+  <si>
+    <t>Fører@@nb | Führer@@de</t>
+  </si>
+  <si>
+    <t>ex:Innførsel</t>
+  </si>
+  <si>
+    <t>Innførsel@@nb</t>
+  </si>
+  <si>
+    <t>ex:Luftfartøy</t>
+  </si>
+  <si>
+    <t>Luftfartøy@@nb | Aircraft@@en</t>
+  </si>
+  <si>
+    <t>ex:Utførsel</t>
+  </si>
+  <si>
+    <t>Utførsel@@nb</t>
+  </si>
+  <si>
+    <t>ex:Vare</t>
+  </si>
+  <si>
+    <t>Vare@@nb | Vare@@nn</t>
+  </si>
+  <si>
+    <t>ex:Definisjon</t>
+  </si>
+  <si>
+    <t>Definisjon@@nb</t>
+  </si>
+  <si>
+    <t>ex:Tollkontroll_Def2</t>
+  </si>
+  <si>
+    <t>ex:World</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +277,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -564,15 +654,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7B1F48-F3C8-43DF-A06E-8CB3E6051372}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
@@ -723,7 +813,215 @@
         <v>36</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BB184981-5AAC-44D3-9D0A-0A4531A535E9}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{AC050769-DB6C-4F62-B9B6-EB03062A2EAA}"/>
@@ -734,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50217266-4028-4AAE-A112-A7883C69CFE0}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,6 +1163,23 @@
         <v>40</v>
       </c>
       <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>